<commit_message>
production shares update MG 0206
</commit_message>
<xml_diff>
--- a/Plotting/production_shares_ammonia.xlsx
+++ b/Plotting/production_shares_ammonia.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,53 +597,53 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1109438.798895803</v>
+        <v>919181.254081609</v>
       </c>
       <c r="C7" t="n">
-        <v>409735.7389518141</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1178222.42760983</v>
+        <v>1001764.273984157</v>
       </c>
       <c r="E7" t="n">
-        <v>1109438.798895803</v>
+        <v>995260.6156279875</v>
       </c>
       <c r="F7" t="n">
-        <v>1179659.189307506</v>
+        <v>933827.17285387</v>
       </c>
       <c r="G7" t="n">
-        <v>1178475.59246352</v>
+        <v>935633.1133170046</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>CO$_2$ utilization</t>
+          <t>Water electrolysis</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>190257.5448141939</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>409735.7389518141</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>176458.1536256725</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>114178.1832678152</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>245832.0164536356</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>242842.4791465157</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Bio-based feedstock</t>
+          <t>CO$_2$ utilization</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -668,7 +668,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Plastic waste recycling</t>
+          <t>Bio-based feedstock</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -693,25 +693,50 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>Plastic waste recycling</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
           <t>Plastic waste recycling with CC</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>